<commit_message>
Aanpassingen requirements + tijdschema
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anastasia\XAMPP\htdocs\NerdyGadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD5F67C-A7F7-42E2-87C2-1D5A0C757E4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{839D22EC-A20F-4CD1-A369-3FFFC8AFA07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projectlid1" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Nog te besteden:</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Jasper in 't Veld</t>
   </si>
   <si>
@@ -124,6 +121,21 @@
   </si>
   <si>
     <t>Les + interview hoofd-sales</t>
+  </si>
+  <si>
+    <t>Jeremy</t>
+  </si>
+  <si>
+    <t>Vermeulen</t>
+  </si>
+  <si>
+    <t>Requirements verwerkt</t>
+  </si>
+  <si>
+    <t>Sales geïnterviewd</t>
+  </si>
+  <si>
+    <t>KSB op locatie</t>
   </si>
 </sst>
 </file>
@@ -218,9 +230,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -238,6 +250,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D45" totalsRowShown="0">
   <autoFilter ref="A9:D45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D45">
+    <sortCondition ref="B9:B45"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Datum"/>
@@ -314,7 +329,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -636,14 +651,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" hidden="1"/>
@@ -662,18 +677,27 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1"/>
@@ -684,7 +708,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>0</v>
+        <v>6.166666666666667</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -696,7 +720,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>168</v>
+        <v>161.83333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -717,6 +741,83 @@
       </c>
       <c r="D9" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44090</v>
+      </c>
+      <c r="C10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44090</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44095</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44095</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44097</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3">
+        <v>44097</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44098</v>
+      </c>
+      <c r="C16">
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -776,7 +877,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -784,7 +885,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -841,10 +942,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="C10">
         <v>60</v>
@@ -852,10 +953,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>60</v>
@@ -863,10 +964,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>60</v>
@@ -1015,7 +1116,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C13" sqref="A10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -1040,7 +1141,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1048,7 +1149,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1105,7 +1206,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>44090</v>
@@ -1116,7 +1217,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>44090</v>
@@ -1127,7 +1228,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>44095</v>
@@ -1138,7 +1239,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3">
         <v>44095</v>
@@ -1204,7 +1305,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1212,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1269,7 +1370,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>44090</v>
@@ -1280,7 +1381,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>44095</v>
@@ -1291,7 +1392,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>44095</v>
@@ -1332,14 +1433,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" hidden="1"/>
@@ -1358,7 +1459,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1366,7 +1467,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1423,7 +1524,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3">
         <v>44090</v>
@@ -1434,7 +1535,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="3">
         <v>44090</v>
@@ -1445,7 +1546,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="3">
         <v>44095</v>
@@ -1456,7 +1557,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="3">
         <v>44095</v>
@@ -1467,7 +1568,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3">
         <v>44097</v>
@@ -1505,6 +1606,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1730,15 +1840,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -1750,6 +1851,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1769,14 +1878,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
weekverslag week 4 gemaakt
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122FCDBA-983C-4BCB-A404-80718EE6B72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320F8165-4B2D-442C-9F12-4C880DEB8BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1680" windowWidth="25440" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Jeremy" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="52">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -724,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1356,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFC46"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D27"/>
+    <sheetView view="pageLayout" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>13.416666666666666</v>
+        <v>13.666666666666666</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>154.58333333333334</v>
+        <v>154.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1654,6 +1654,17 @@
       </c>
       <c r="D27" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="3">
+        <v>44106</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1687,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D20"/>
+    <sheetView view="pageLayout" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
@@ -1935,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D27"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
@@ -1989,7 +2000,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>12.916666666666666</v>
+        <v>13.166666666666666</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2001,7 +2012,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>155.08333333333334</v>
+        <v>154.83333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2223,6 +2234,17 @@
       </c>
       <c r="D27" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="3">
+        <v>44106</v>
+      </c>
+      <c r="C28">
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2254,15 +2276,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2488,6 +2501,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -2499,14 +2521,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2522,6 +2536,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update Jeremy en Ivar
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564AB11D-11BD-4AAC-9B77-4CC880D78CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD490EAB-1AE6-4FAD-97AB-BE22D52F4B30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="58">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>De lijst met conversie verhogende maatregelen uitgewerkt.</t>
+  </si>
+  <si>
+    <t>les KBS</t>
+  </si>
+  <si>
+    <t>Gastcolleges bekeken en aantekingen gemaakt</t>
+  </si>
+  <si>
+    <t>Verder werken aan conversiemaatregelen</t>
+  </si>
+  <si>
+    <t>Afmaken conversiemaatregelen</t>
   </si>
 </sst>
 </file>
@@ -731,7 +743,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
@@ -787,7 +799,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>7.666666666666667</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -799,7 +811,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>160.33333333333334</v>
+        <v>155</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -930,6 +942,61 @@
       </c>
       <c r="C19">
         <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="3">
+        <v>44111</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="3">
+        <v>44112</v>
+      </c>
+      <c r="C21">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="3">
+        <v>44112</v>
+      </c>
+      <c r="C22">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="3">
+        <v>44116</v>
+      </c>
+      <c r="C23">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="3">
+        <v>44117</v>
+      </c>
+      <c r="C24">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -963,7 +1030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
@@ -1360,7 +1427,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:XFD46"/>
+  <dimension ref="A1:XFC46"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
@@ -1417,7 +1484,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>16.166666666666668</v>
+        <v>17.083333333333332</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1429,7 +1496,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>151.83333333333334</v>
+        <v>150.91666666666666</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1540,7 +1607,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="57.6">
+    <row r="18" spans="1:4" ht="43.2">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -1685,6 +1752,28 @@
       </c>
       <c r="D29" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="3">
+        <v>44117</v>
+      </c>
+      <c r="C30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="3">
+        <v>44112</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1967,7 +2056,7 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:C28"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
@@ -2296,15 +2385,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2530,6 +2610,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -2541,14 +2630,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2564,6 +2645,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
logboek en verbrokenregels aangepast
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anastasia\XAMPP\htdocs\NerdyGadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEE1A6F-4A14-41D8-99D7-A0671EB0BC81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15218D6E-B54B-4608-8A97-E60A1273D3E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Jeremy" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="68">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>Begin functioneel ontwerp</t>
+  </si>
+  <si>
+    <t>Functioneel ontwerp</t>
+  </si>
+  <si>
+    <t>Schermontwerp</t>
+  </si>
+  <si>
+    <t>Domeinmodel</t>
   </si>
 </sst>
 </file>
@@ -342,9 +351,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -441,7 +450,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -763,7 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2240,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:XFC46"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:C34"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2295,7 +2304,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>23.5</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2307,7 +2316,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>144.5</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2618,6 +2627,45 @@
       </c>
       <c r="C34">
         <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="3">
+        <v>44130</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="3">
+        <v>44132</v>
+      </c>
+      <c r="C36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="3">
+        <v>44134</v>
+      </c>
+      <c r="C37">
+        <v>120</v>
+      </c>
+      <c r="D37" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2649,6 +2697,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2874,15 +2931,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -2894,6 +2942,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2909,14 +2965,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Logboek geüpate, opzet toevoegen aan winkelwagen
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D90352C-6122-4788-82C6-0342C95A924E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204ED06C-14BA-421D-98E9-8517955EE3E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="85">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>Bekeken waar het in view.php gezet moet worden. De knop gemaakt en op de goede plek gezet. Is nog niet optimaal gekeken naar opmaak</t>
+  </si>
+  <si>
+    <t>Probleem oplossen toevoegen aan winkelwagen</t>
+  </si>
+  <si>
+    <t>Probleem: Het toevoegen werkt niet. Dit is opgelost. Daarna was er een nieuw probleem: Je kan niet meer dan 1 item toevoegen. Dit kwam omdat het aantal een string was en we konden er geen integer van maken. Dit is bijna opgelost, alleen uit het functioneel ontwerp is gebleken dat we dit alleen moeten doen bij het aanpassen van de winkelmand.</t>
   </si>
 </sst>
 </file>
@@ -369,7 +375,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -394,6 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1693,7 +1700,7 @@
   <dimension ref="A1:XFC46"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -1747,7 +1754,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>40.166666666666664</v>
+        <v>42.166666666666664</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1759,7 +1766,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>127.83333333333334</v>
+        <v>125.83333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2213,9 +2220,18 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="12">
+        <v>44146</v>
+      </c>
+      <c r="C45" s="2">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2"/>
@@ -2660,7 +2676,7 @@
   <dimension ref="A1:XFC46"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="D45" sqref="A45:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2714,7 +2730,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>37.5</v>
+        <v>39.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2726,7 +2742,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>130.5</v>
+        <v>128.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3168,9 +3184,18 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="12">
+        <v>44146</v>
+      </c>
+      <c r="C45" s="2">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2"/>
@@ -3206,6 +3231,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3431,15 +3465,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
   <ds:schemaRefs>
@@ -3459,6 +3484,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3476,12 +3509,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Logo en knop naar winkelwagen toegevoegd.
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204ED06C-14BA-421D-98E9-8517955EE3E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3E1827-744A-445E-A86F-915E3B5BA7BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="87">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>Probleem: Het toevoegen werkt niet. Dit is opgelost. Daarna was er een nieuw probleem: Je kan niet meer dan 1 item toevoegen. Dit kwam omdat het aantal een string was en we konden er geen integer van maken. Dit is bijna opgelost, alleen uit het functioneel ontwerp is gebleken dat we dit alleen moeten doen bij het aanpassen van de winkelmand.</t>
+  </si>
+  <si>
+    <t>Verder gegaan toevoegen aan winkelwagen</t>
+  </si>
+  <si>
+    <t>Knop ga naar winkelwagen toegevoegd. Voeg toe aan winkelwagen knop voegt nu 1 item toe en geeft meldingen op basis van of het er al in staat of niet. Logo toegevoegd</t>
   </si>
 </sst>
 </file>
@@ -394,13 +400,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -489,8 +495,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D45" totalsRowShown="0">
-  <autoFilter ref="A9:D45" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D46" totalsRowShown="0">
+  <autoFilter ref="A9:D46" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -838,12 +844,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -1203,12 +1209,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -1602,12 +1608,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -1714,12 +1720,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -2223,7 +2229,7 @@
       <c r="A45" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="10">
         <v>44146</v>
       </c>
       <c r="C45" s="2">
@@ -2273,12 +2279,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -2676,7 +2682,7 @@
   <dimension ref="A1:XFC46"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D45" sqref="A45:D45"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2690,12 +2696,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
@@ -2730,7 +2736,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>39.5</v>
+        <v>40.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2742,7 +2748,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>128.5</v>
+        <v>127.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3187,7 +3193,7 @@
       <c r="A45" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="10">
         <v>44146</v>
       </c>
       <c r="C45" s="2">
@@ -3198,10 +3204,18 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="10">
+        <v>44146</v>
+      </c>
+      <c r="C46" s="2">
+        <v>60</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3231,15 +3245,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3465,6 +3470,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
   <ds:schemaRefs>
@@ -3484,14 +3498,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3509,4 +3515,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Toevoegen aan winkelwagen is af
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janwillem/.bitnami/stackman/machines/xampp/volumes/root/htdocs/Nerdygadgets/Documenten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1820766-C388-0446-800F-3635056B74F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4987C0DC-BC58-4471-BC04-FB20C9C466B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Jeremy" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="93">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -310,13 +310,25 @@
   </si>
   <si>
     <t>De cookies worden opgehaald vanaf view.php</t>
+  </si>
+  <si>
+    <t>Jan Willem geholpen een begin te maken</t>
+  </si>
+  <si>
+    <t>Geholpen met het begrijpen van html en css</t>
+  </si>
+  <si>
+    <t>Laatste stukje afgemaakt toevoegen aan winkelwagen</t>
+  </si>
+  <si>
+    <t>Knop wordt nu grijs als er geen items meer op voorraad zijn. We zijn weer teruggestapt naar sessievariabelen want het opslaan van een array in een cookie werkte niet zoals we verwacht hadden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,8 +513,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D46" totalsRowShown="0">
-  <autoFilter ref="A9:D46" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D48" totalsRowShown="0">
+  <autoFilter ref="A9:D48" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -840,16 +852,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -857,7 +869,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -868,7 +880,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -876,7 +888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -884,10 +896,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -899,7 +911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -911,10 +923,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -928,7 +940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -939,7 +951,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -950,7 +962,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -961,7 +973,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -972,7 +984,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -983,7 +995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1005,7 +1017,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1016,7 +1028,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1027,7 +1039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1049,7 +1061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1071,7 +1083,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1082,7 +1094,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1093,7 +1105,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1104,7 +1116,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1115,7 +1127,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -1137,7 +1149,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -1148,7 +1160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1159,7 +1171,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -1170,12 +1182,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1201,20 +1213,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A3" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" hidden="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1234,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1230,7 +1242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1250,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1246,10 +1258,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1261,7 +1273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1273,10 +1285,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -1312,7 +1324,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1335,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1356,7 +1368,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1389,7 +1401,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1400,7 +1412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1411,7 +1423,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1422,7 +1434,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1433,7 +1445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1444,7 +1456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1486,7 +1498,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1500,7 +1512,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -1514,7 +1526,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -1525,7 +1537,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -1536,7 +1548,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -1547,7 +1559,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1558,7 +1570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -1569,7 +1581,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1591,7 +1603,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -1602,12 +1614,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1637,16 +1649,16 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1654,25 +1666,25 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1696,10 +1708,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1713,12 +1725,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1748,17 +1760,17 @@
       <selection activeCell="A41" sqref="A41:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="16383" width="9.1640625" hidden="1"/>
-    <col min="16384" max="16384" width="0.1640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="16383" width="9.140625" hidden="1"/>
+    <col min="16384" max="16384" width="0.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1778,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1774,7 +1786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1790,10 +1802,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1805,7 +1817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1817,10 +1829,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1834,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -1845,7 +1857,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
@@ -1856,7 +1868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -1867,7 +1879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
         <v>16</v>
       </c>
@@ -1878,7 +1890,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
@@ -1889,7 +1901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
@@ -1900,7 +1912,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
         <v>27</v>
       </c>
@@ -1911,7 +1923,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="45">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
@@ -1936,7 +1948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="30">
       <c r="A19" s="7" t="s">
         <v>45</v>
       </c>
@@ -1950,7 +1962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
         <v>47</v>
       </c>
@@ -1964,7 +1976,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -1975,7 +1987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
         <v>41</v>
       </c>
@@ -1986,7 +1998,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
@@ -1997,7 +2009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
         <v>42</v>
       </c>
@@ -2008,7 +2020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2019,7 +2031,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2030,7 +2042,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -2044,7 +2056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2055,7 +2067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -2069,7 +2081,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -2091,7 +2103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -2105,7 +2117,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -2119,7 +2131,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -2133,7 +2145,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -2147,7 +2159,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -2172,7 +2184,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -2186,7 +2198,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2197,7 +2209,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -2208,7 +2220,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -2222,7 +2234,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2236,7 +2248,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -2250,7 +2262,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2264,7 +2276,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>83</v>
       </c>
@@ -2278,7 +2290,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>87</v>
       </c>
@@ -2316,16 +2328,16 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2333,7 +2345,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2341,7 +2353,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2357,10 +2369,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2384,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -2384,10 +2396,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2401,7 +2413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2412,7 +2424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2423,7 +2435,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
@@ -2434,7 +2446,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2445,7 +2457,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -2456,7 +2468,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2467,7 +2479,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2489,7 +2501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2500,7 +2512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2511,7 +2523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -2522,7 +2534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -2533,7 +2545,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2544,7 +2556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2555,7 +2567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -2569,7 +2581,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2583,7 +2595,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -2597,7 +2609,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -2611,7 +2623,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>62</v>
       </c>
@@ -2625,7 +2637,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -2636,7 +2648,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -2647,7 +2659,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>70</v>
       </c>
@@ -2658,7 +2670,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2669,7 +2681,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -2680,28 +2692,28 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="9"/>
       <c r="B38" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2726,23 +2738,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:XFC46"/>
+  <dimension ref="A1:XFC48"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
     <col min="5" max="16383" width="0" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="7.5" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="7.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2750,7 +2762,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -2758,7 +2770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2766,7 +2778,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2774,37 +2786,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>40.5</v>
+        <v>44.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>127.5</v>
+        <v>123.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="24.75" customHeight="1">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -2818,7 +2830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2829,7 +2841,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2840,7 +2852,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2851,7 +2863,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -2862,7 +2874,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2873,7 +2885,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2884,7 +2896,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2895,7 +2907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2906,7 +2918,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2917,7 +2929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2928,7 +2940,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2939,7 +2951,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -2950,7 +2962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -2961,7 +2973,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2972,7 +2984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2983,7 +2995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -3005,7 +3017,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -3019,7 +3031,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -3030,7 +3042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -3044,7 +3056,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -3058,7 +3070,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>42</v>
       </c>
@@ -3069,7 +3081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -3083,7 +3095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>62</v>
       </c>
@@ -3097,7 +3109,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3120,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -3122,7 +3134,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3133,7 +3145,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>65</v>
       </c>
@@ -3147,7 +3159,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -3158,7 +3170,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -3169,7 +3181,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -3180,7 +3192,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -3194,7 +3206,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -3208,7 +3220,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -3222,7 +3234,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -3236,7 +3248,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>83</v>
       </c>
@@ -3250,7 +3262,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>85</v>
       </c>
@@ -3262,6 +3274,34 @@
       </c>
       <c r="D46" s="2" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="3">
+        <v>44147</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="3">
+        <v>44147</v>
+      </c>
+      <c r="C48">
+        <v>195</v>
+      </c>
+      <c r="D48" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -3508,15 +3548,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
@@ -3524,6 +3555,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3547,14 +3587,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3570,4 +3602,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tijschriftformulier en pay.php afgemaakt
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janwillem/.bitnami/stackman/machines/xampp/volumes/root/htdocs/Nerdygadgets/Documenten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE1F9E0-2019-004B-A90B-17DECF42AC2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC6FB45-8323-934A-9EB3-159FBC91CCB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Jeremy" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="98">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -328,6 +328,15 @@
   </si>
   <si>
     <t>order pagina verder gemaakt &amp; begin betaalpagina</t>
+  </si>
+  <si>
+    <t>workshop kbs gevolgd van de kbs docent</t>
+  </si>
+  <si>
+    <t>bezig geweest aan order.php en pay.php</t>
+  </si>
+  <si>
+    <t>heel veel opnieuw gedaan in order.php omdat ik de indeling anders wilde uitgebreide uitleg in mijn eigen logboek.</t>
   </si>
 </sst>
 </file>
@@ -1219,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1273,7 +1282,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>35.666666666666664</v>
+        <v>42.333333333333336</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1285,7 +1294,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>132.33333333333334</v>
+        <v>125.66666666666666</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1640,6 +1649,31 @@
       </c>
       <c r="C38">
         <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="3">
+        <v>44148</v>
+      </c>
+      <c r="C39">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="3">
+        <v>44148</v>
+      </c>
+      <c r="C40">
+        <v>330</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1784,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFC46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3350,25 +3384,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3594,10 +3609,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3621,21 +3667,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tijdschriftform KBS op locatie
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767C467E-8BEA-41B5-B397-9866A215F0CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8227DA4-07F9-414F-B99A-8C1595199A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Jeremy" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="129">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -567,8 +567,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15723" displayName="Table15723" ref="A9:D45" totalsRowShown="0">
-  <autoFilter ref="A9:D45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15723" displayName="Table15723" ref="A9:D46" totalsRowShown="0">
+  <autoFilter ref="A9:D46" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Datum"/>
@@ -580,8 +580,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1572345" displayName="Table1572345" ref="A9:D56" totalsRowShown="0">
-  <autoFilter ref="A9:D56" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1572345" displayName="Table1572345" ref="A9:D57" totalsRowShown="0">
+  <autoFilter ref="A9:D57" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Datum"/>
@@ -606,8 +606,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D54" totalsRowShown="0">
-  <autoFilter ref="A9:D54" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D55" totalsRowShown="0">
+  <autoFilter ref="A9:D55" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -941,20 +941,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A20" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A20" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:4" ht="25.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1427,19 +1427,19 @@
   <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:D45"/>
+      <selection activeCell="A46" sqref="A46:D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.140625" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:4" ht="25.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>50.166666666666664</v>
+        <v>53.666666666666664</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>117.83333333333334</v>
+        <v>114.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1942,9 +1942,15 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="A46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="10">
+        <v>44154</v>
+      </c>
+      <c r="C46" s="2">
+        <v>210</v>
+      </c>
       <c r="D46" s="2"/>
     </row>
   </sheetData>
@@ -1965,23 +1971,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:XFC56"/>
+  <dimension ref="A1:XFC57"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:D56"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="16383" width="9.140625" hidden="1"/>
-    <col min="16384" max="16384" width="0.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="5" max="16383" width="9.109375" hidden="1"/>
+    <col min="16384" max="16384" width="0.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:4" ht="25.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2028,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C154)/60</f>
-        <v>62.25</v>
+        <v>65.75</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2034,7 +2040,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C154)/60)</f>
-        <v>105.75</v>
+        <v>102.25</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2145,7 +2151,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="45">
+    <row r="18" spans="1:4" ht="43.2">
       <c r="A18" s="7" t="s">
         <v>45</v>
       </c>
@@ -2159,7 +2165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30">
+    <row r="19" spans="1:4" ht="28.8">
       <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
@@ -2342,7 +2348,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30">
+    <row r="34" spans="1:4" ht="28.8">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -2648,6 +2654,18 @@
       <c r="D56" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="10">
+        <v>44154</v>
+      </c>
+      <c r="C57" s="2">
+        <v>210</v>
+      </c>
+      <c r="D57" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2669,20 +2687,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:D42"/>
+    <sheetView view="pageLayout" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:4" ht="25.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2723,7 +2741,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>43.166666666666664</v>
+        <v>46.666666666666664</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2735,7 +2753,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>124.83333333333334</v>
+        <v>121.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3156,6 +3174,18 @@
       <c r="D42" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43" s="10">
+        <v>44154</v>
+      </c>
+      <c r="C43" s="2">
+        <v>210</v>
+      </c>
+      <c r="D43" s="2"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2"/>
@@ -3187,23 +3217,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:XFC54"/>
+  <dimension ref="A1:XFC55"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:D54"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" customWidth="1"/>
     <col min="5" max="16383" width="0" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="7.42578125" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="7.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:4" ht="25.8">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3244,7 +3274,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>54.5</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3256,7 +3286,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>113.5</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3833,6 +3863,18 @@
       <c r="D54" t="s">
         <v>128</v>
       </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="10">
+        <v>44154</v>
+      </c>
+      <c r="C55" s="2">
+        <v>210</v>
+      </c>
+      <c r="D55" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3852,6 +3894,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4077,26 +4138,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4114,30 +4182,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tijdformulier (auto-data invullen werkt niet)
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anastasia\XAMPP\htdocs\NerdyGadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A85B8D6-1CCE-4952-A4E4-B759C2F70F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A673AD1-2CF9-4813-BFDA-D5D8144951BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
     <sheet name="P2 - Jan Willem" sheetId="8" r:id="rId2"/>
-    <sheet name="P4 - Ivar" sheetId="10" r:id="rId3"/>
-    <sheet name="P5 - Roy" sheetId="11" r:id="rId4"/>
-    <sheet name="P6 - Jasper" sheetId="6" r:id="rId5"/>
+    <sheet name="P3 - Ivar" sheetId="10" r:id="rId3"/>
+    <sheet name="P4 - Roy" sheetId="11" r:id="rId4"/>
+    <sheet name="P5 - Jasper" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'P1 - Anastasia'!$A$1:$D$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'P2 - Jan Willem'!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'P4 - Ivar'!$A$1:$D$48</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'P5 - Roy'!$A$1:$D$47</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'P6 - Jasper'!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'P3 - Ivar'!$A$1:$D$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'P4 - Roy'!$A$1:$D$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'P5 - Jasper'!$A$1:$D$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="135">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Weekverslag ingevuld</t>
   </si>
   <si>
-    <t>31-9-2020</t>
-  </si>
-  <si>
     <t>Onvolledige database, onjuist Testplan. 1-10-2020 verbeterd</t>
   </si>
   <si>
@@ -440,6 +437,15 @@
   </si>
   <si>
     <t>Anastasia</t>
+  </si>
+  <si>
+    <t>Demo doorgelopen</t>
+  </si>
+  <si>
+    <t>Met Ivar demo extra doorgegaan</t>
+  </si>
+  <si>
+    <t>31/9/2020</t>
   </si>
 </sst>
 </file>
@@ -592,8 +598,11 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1572345" displayName="Table1572345" ref="A9:D59" totalsRowShown="0">
-  <autoFilter ref="A9:D59" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1572345" displayName="Table1572345" ref="A9:D67" totalsRowShown="0">
+  <autoFilter ref="A9:D67" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D67">
+    <sortCondition ref="B9:B67"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Datum"/>
@@ -953,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView view="pageLayout" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -979,7 +988,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -1010,7 +1019,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>42.166666666666664</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1022,7 +1031,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>125.83333333333334</v>
+        <v>125.33333333333334</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1168,7 +1177,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3">
         <v>44112</v>
@@ -1179,7 +1188,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3">
         <v>44112</v>
@@ -1190,7 +1199,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3">
         <v>44116</v>
@@ -1201,7 +1210,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3">
         <v>44117</v>
@@ -1223,7 +1232,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="3">
         <v>44126</v>
@@ -1234,7 +1243,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" s="3">
         <v>44127</v>
@@ -1245,7 +1254,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" s="3">
         <v>44134</v>
@@ -1256,7 +1265,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="3">
         <v>44134</v>
@@ -1267,7 +1276,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="3">
         <v>44136</v>
@@ -1278,7 +1287,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3">
         <v>44136</v>
@@ -1289,7 +1298,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="3">
         <v>44141</v>
@@ -1298,12 +1307,12 @@
         <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3">
         <v>44144</v>
@@ -1312,12 +1321,12 @@
         <v>60</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3">
         <v>44145</v>
@@ -1326,7 +1335,7 @@
         <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1342,7 +1351,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B36" s="3">
         <v>44149</v>
@@ -1351,12 +1360,12 @@
         <v>150</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="3">
         <v>44150</v>
@@ -1365,12 +1374,12 @@
         <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="3">
         <v>44151</v>
@@ -1381,30 +1390,44 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="B39" s="3">
-        <v>44153</v>
+        <v>44151</v>
       </c>
       <c r="C39">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B40" s="3">
         <v>44153</v>
       </c>
       <c r="C40">
+        <v>60</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="3">
+        <v>44153</v>
+      </c>
+      <c r="C41">
         <v>80</v>
       </c>
-      <c r="D40" t="s">
-        <v>127</v>
+      <c r="D41" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1683,7 +1706,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="3">
         <v>44112</v>
@@ -1692,12 +1715,12 @@
         <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3">
         <v>44116</v>
@@ -1706,12 +1729,12 @@
         <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3">
         <v>44117</v>
@@ -1720,7 +1743,7 @@
         <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1734,12 +1757,12 @@
         <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3">
         <v>44126</v>
@@ -1748,12 +1771,12 @@
         <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3">
         <v>44127</v>
@@ -1764,7 +1787,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3">
         <v>44134</v>
@@ -1775,7 +1798,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3">
         <v>44134</v>
@@ -1786,7 +1809,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3">
         <v>44136</v>
@@ -1797,7 +1820,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="3">
         <v>44136</v>
@@ -1808,7 +1831,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="3">
         <v>44141</v>
@@ -1819,7 +1842,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="3">
         <v>44113</v>
@@ -1830,7 +1853,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B36" s="3">
         <v>44145</v>
@@ -1841,7 +1864,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" s="3">
         <v>44147</v>
@@ -1852,7 +1875,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" s="3">
         <v>44147</v>
@@ -1863,7 +1886,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" s="3">
         <v>44148</v>
@@ -1874,7 +1897,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B40" s="3">
         <v>44148</v>
@@ -1883,12 +1906,12 @@
         <v>330</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B41" s="3">
         <v>44149</v>
@@ -1897,12 +1920,12 @@
         <v>60</v>
       </c>
       <c r="D41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B42" s="3">
         <v>44151</v>
@@ -1913,7 +1936,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" s="3">
         <v>44152</v>
@@ -1922,12 +1945,12 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B44" s="3">
         <v>44153</v>
@@ -1936,12 +1959,12 @@
         <v>60</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B45" s="3">
         <v>44153</v>
@@ -1950,7 +1973,7 @@
         <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1983,10 +2006,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:XFC59"/>
+  <dimension ref="A1:XFC60"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -2040,7 +2063,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C154)/60</f>
-        <v>68.083333333333329</v>
+        <v>68.583333333333329</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2052,7 +2075,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C154)/60)</f>
-        <v>99.916666666666671</v>
+        <v>99.416666666666671</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2165,7 +2188,7 @@
     </row>
     <row r="18" spans="1:4" ht="45">
       <c r="A18" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="3">
         <v>44104</v>
@@ -2179,21 +2202,21 @@
     </row>
     <row r="19" spans="1:4" ht="30">
       <c r="A19" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="C19">
         <v>15</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="8">
         <v>44105</v>
@@ -2202,7 +2225,7 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2262,7 +2285,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3">
         <v>44111</v>
@@ -2273,7 +2296,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3">
         <v>44112</v>
@@ -2282,7 +2305,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2298,7 +2321,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29" s="3">
         <v>44116</v>
@@ -2307,12 +2330,12 @@
         <v>150</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="3">
         <v>44117</v>
@@ -2343,12 +2366,12 @@
         <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3">
         <v>44126</v>
@@ -2357,12 +2380,12 @@
         <v>195</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="3">
         <v>44127</v>
@@ -2371,12 +2394,12 @@
         <v>275</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="3">
         <v>44127</v>
@@ -2385,12 +2408,12 @@
         <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" s="3">
         <v>44130</v>
@@ -2399,7 +2422,7 @@
         <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2415,7 +2438,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="3">
         <v>44134</v>
@@ -2424,12 +2447,12 @@
         <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3">
         <v>44134</v>
@@ -2440,7 +2463,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="3">
         <v>44136</v>
@@ -2451,7 +2474,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="3">
         <v>44141</v>
@@ -2460,12 +2483,12 @@
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" s="3">
         <v>44144</v>
@@ -2474,12 +2497,12 @@
         <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="3">
         <v>44145</v>
@@ -2488,12 +2511,12 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="3">
         <v>44145</v>
@@ -2502,12 +2525,12 @@
         <v>180</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="10">
         <v>44146</v>
@@ -2516,12 +2539,12 @@
         <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="10">
         <v>44146</v>
@@ -2530,7 +2553,7 @@
         <v>60</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2546,7 +2569,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B48" s="3">
         <v>44148</v>
@@ -2555,12 +2578,12 @@
         <v>120</v>
       </c>
       <c r="D48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" s="3">
         <v>44148</v>
@@ -2569,12 +2592,12 @@
         <v>240</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="3">
         <v>44149</v>
@@ -2583,12 +2606,12 @@
         <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B51" s="3">
         <v>44149</v>
@@ -2597,12 +2620,12 @@
         <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B52" s="3">
         <v>44151</v>
@@ -2613,98 +2636,112 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B53" s="3">
-        <v>44152</v>
+        <v>44151</v>
       </c>
       <c r="C53">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D53" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B54" s="3">
         <v>44152</v>
       </c>
       <c r="C54">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
         <v>120</v>
-      </c>
-      <c r="D54" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B55" s="3">
-        <v>44153</v>
+        <v>44152</v>
       </c>
       <c r="C55">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B56" s="3">
         <v>44153</v>
       </c>
       <c r="C56">
+        <v>60</v>
+      </c>
+      <c r="D56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="3">
+        <v>44153</v>
+      </c>
+      <c r="C57">
         <v>80</v>
       </c>
-      <c r="D56" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="2" t="s">
+      <c r="D57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B57" s="10">
+      <c r="B58" s="10">
         <v>44154</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C58" s="2">
         <v>210</v>
       </c>
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" t="s">
-        <v>128</v>
-      </c>
-      <c r="B58" s="3">
-        <v>44154</v>
-      </c>
-      <c r="C58">
-        <v>20</v>
-      </c>
-      <c r="D58" t="s">
-        <v>129</v>
-      </c>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B59" s="3">
         <v>44154</v>
       </c>
       <c r="C59">
+        <v>20</v>
+      </c>
+      <c r="D59" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" s="3">
+        <v>44154</v>
+      </c>
+      <c r="C60">
         <v>120</v>
       </c>
-      <c r="D59" t="s">
-        <v>131</v>
+      <c r="D60" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2821,7 +2858,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10">
         <v>60</v>
@@ -2832,7 +2869,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11">
         <v>60</v>
@@ -2843,7 +2880,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12">
         <v>60</v>
@@ -2854,7 +2891,7 @@
         <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -2865,7 +2902,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14">
         <v>30</v>
@@ -2876,7 +2913,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15">
         <v>70</v>
@@ -2887,7 +2924,7 @@
         <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16">
         <v>40</v>
@@ -2898,7 +2935,7 @@
         <v>35</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -2909,7 +2946,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -2920,7 +2957,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19">
         <v>10</v>
@@ -2972,7 +3009,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="3">
         <v>44053</v>
@@ -2981,12 +3018,12 @@
         <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3">
         <v>44175</v>
@@ -2995,21 +3032,21 @@
         <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C26">
         <v>40</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3017,35 +3054,35 @@
         <v>30</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27">
         <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C28">
         <v>195</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29">
         <v>275</v>
@@ -3053,10 +3090,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30">
         <v>120</v>
@@ -3064,10 +3101,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31">
         <v>120</v>
@@ -3075,7 +3112,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="3">
         <v>43841</v>
@@ -3086,7 +3123,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3">
         <v>43993</v>
@@ -3095,12 +3132,12 @@
         <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="3">
         <v>44085</v>
@@ -3109,12 +3146,12 @@
         <v>60</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="3">
         <v>44115</v>
@@ -3123,12 +3160,12 @@
         <v>60</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" s="3">
         <v>44146</v>
@@ -3137,12 +3174,12 @@
         <v>120</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="3">
         <v>44176</v>
@@ -3153,24 +3190,24 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38">
         <v>70</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39">
         <v>150</v>
@@ -3178,7 +3215,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B40" s="3">
         <v>44151</v>
@@ -3189,7 +3226,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" s="3">
         <v>44153</v>
@@ -3198,12 +3235,12 @@
         <v>60</v>
       </c>
       <c r="D41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" s="3">
         <v>44153</v>
@@ -3212,7 +3249,7 @@
         <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3260,7 +3297,7 @@
   <dimension ref="A1:XFC55"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:D55"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3527,7 +3564,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26" s="3">
         <v>44111</v>
@@ -3538,7 +3575,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="3">
         <v>44112</v>
@@ -3547,7 +3584,7 @@
         <v>45</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3563,7 +3600,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="3">
         <v>44116</v>
@@ -3572,12 +3609,12 @@
         <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="3">
         <v>44117</v>
@@ -3586,7 +3623,7 @@
         <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -3611,12 +3648,12 @@
         <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3">
         <v>44126</v>
@@ -3625,12 +3662,12 @@
         <v>195</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="3">
         <v>44127</v>
@@ -3641,7 +3678,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="3">
         <v>44130</v>
@@ -3650,7 +3687,7 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3666,7 +3703,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" s="3">
         <v>44134</v>
@@ -3675,12 +3712,12 @@
         <v>120</v>
       </c>
       <c r="D37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="3">
         <v>44134</v>
@@ -3691,7 +3728,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="3">
         <v>44136</v>
@@ -3702,7 +3739,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="3">
         <v>44136</v>
@@ -3713,7 +3750,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B41" s="3">
         <v>44141</v>
@@ -3722,12 +3759,12 @@
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B42" s="3">
         <v>44113</v>
@@ -3736,12 +3773,12 @@
         <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" s="3">
         <v>44145</v>
@@ -3750,12 +3787,12 @@
         <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="3">
         <v>44145</v>
@@ -3764,12 +3801,12 @@
         <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="10">
         <v>44146</v>
@@ -3778,12 +3815,12 @@
         <v>120</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="10">
         <v>44146</v>
@@ -3792,12 +3829,12 @@
         <v>60</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" s="3">
         <v>44147</v>
@@ -3806,12 +3843,12 @@
         <v>45</v>
       </c>
       <c r="D47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="3">
         <v>44147</v>
@@ -3820,12 +3857,12 @@
         <v>195</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B49" s="3">
         <v>44148</v>
@@ -3834,12 +3871,12 @@
         <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" s="3">
         <v>44148</v>
@@ -3848,12 +3885,12 @@
         <v>120</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B51" s="3">
         <v>44151</v>
@@ -3864,7 +3901,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B52" s="3">
         <v>44152</v>
@@ -3873,12 +3910,12 @@
         <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="3">
         <v>44153</v>
@@ -3887,12 +3924,12 @@
         <v>60</v>
       </c>
       <c r="D53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B54" s="3">
         <v>44153</v>
@@ -3901,7 +3938,7 @@
         <v>80</v>
       </c>
       <c r="D54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:4">

</xml_diff>

<commit_message>
Login page werkend + logboek
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\NerdyGadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4824F6-ECE7-4D77-8576-4339DB529143}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918F0605-F41D-484A-9899-DFAFC4E2F8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="161">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -518,6 +518,12 @@
   </si>
   <si>
     <t>Bedrag kan ingevoerd worden maar het controleren ervan in confirmation.php gebeurt nog niet.</t>
+  </si>
+  <si>
+    <t>De vraag was hoe je het controleren voor het kloppen van het wachtwoord en het al bestaan van het emailadres kon doen. Beetje met sweetalert gewerkt met Ivar. Uiteindelijk was het antwoord dat het niet kon op de manier die ik nu had (alles op 1 pagina en laten zien dmv posts). Besloten om later 3 verschillende pagina's te maken.</t>
+  </si>
+  <si>
+    <t>De 3 pagina's gemaakt. Het controleren gebeurt nu in hetzelfde bestand, en je wordt niet meer doorgestuurd door het formulier. Dit wordt gedaan door de functie header(), maar dit is minder goed voor de security. Verder besloten de velden behalve het wachtwoord gevuld te laten wanneer er een foutmelding kwam. Ook is de functionaliteit voor de inlogpagina gemaakt en bestaat er een sessie account na het succesvol inloggen.</t>
   </si>
 </sst>
 </file>
@@ -699,8 +705,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D62" totalsRowShown="0">
-  <autoFilter ref="A9:D62" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D64" totalsRowShown="0">
+  <autoFilter ref="A9:D64" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -1592,7 +1598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A31" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
@@ -3523,10 +3529,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:XFC62"/>
+  <dimension ref="A1:XFC64"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3580,7 +3586,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C153)/60</f>
-        <v>70.083333333333329</v>
+        <v>75.583333333333329</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3592,7 +3598,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C153)/60)</f>
-        <v>97.916666666666671</v>
+        <v>92.416666666666671</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4275,6 +4281,34 @@
       </c>
       <c r="C62">
         <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>139</v>
+      </c>
+      <c r="B63" s="3">
+        <v>44158</v>
+      </c>
+      <c r="C63">
+        <v>90</v>
+      </c>
+      <c r="D63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="3">
+        <v>44161</v>
+      </c>
+      <c r="C64">
+        <v>240</v>
+      </c>
+      <c r="D64" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -4295,6 +4329,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4520,26 +4573,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4557,30 +4617,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
export pdf + Css + tijdschriftformulier
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\nerdygadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets-master\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8361C8D0-58BF-4BF1-AB01-3D24AF28CAB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8801A91B-E97B-4722-861D-713BD50DD3FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="199">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -611,6 +611,33 @@
   </si>
   <si>
     <t>PDF geintegreerd met het systeem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Export PDF </t>
+  </si>
+  <si>
+    <t>PDF document css</t>
+  </si>
+  <si>
+    <t>afronden pdf en begin css</t>
+  </si>
+  <si>
+    <t>Css leren</t>
+  </si>
+  <si>
+    <t>online informatie opzoeken en begin maken</t>
+  </si>
+  <si>
+    <t>zelf proberen te stylen</t>
+  </si>
+  <si>
+    <t>Pdf document afgerond en gestyled</t>
+  </si>
+  <si>
+    <t>Hulp gekregen van Ivar met wat start problemen</t>
+  </si>
+  <si>
+    <t>Afronden PDF document</t>
   </si>
 </sst>
 </file>
@@ -688,7 +715,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -714,11 +741,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -779,8 +807,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15723456" displayName="Table15723456" ref="A9:D49" totalsRowShown="0">
-  <autoFilter ref="A9:D49" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15723456" displayName="Table15723456" ref="A9:D54" totalsRowShown="0">
+  <autoFilter ref="A9:D54" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Datum"/>
@@ -805,7 +833,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1127,20 +1155,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A43" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A25" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1760,20 +1788,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A34" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A53" sqref="A53:C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.109375" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2396,21 +2424,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFC72"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A55" workbookViewId="0">
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="16383" width="9.109375" hidden="1"/>
-    <col min="16384" max="16384" width="0.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="16383" width="9.140625" hidden="1"/>
+    <col min="16384" max="16384" width="0.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2574,7 +2602,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2">
+    <row r="18" spans="1:4" ht="45">
       <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
@@ -2588,7 +2616,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8">
+    <row r="19" spans="1:4" ht="30">
       <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
@@ -2771,7 +2799,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.8">
+    <row r="34" spans="1:4" ht="30">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3309,22 +3337,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:C49"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -3364,8 +3392,8 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <f>SUM(C10:C152)/60</f>
-        <v>56.083333333333336</v>
+        <f>SUM(C10:C154)/60</f>
+        <v>63.25</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3376,8 +3404,8 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>111.91666666666666</v>
+        <f>(2*3*28)-(SUM(C10:C154)/60)</f>
+        <v>104.75</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3870,7 +3898,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>172</v>
       </c>
@@ -3879,6 +3907,76 @@
       </c>
       <c r="C49">
         <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="13">
+        <v>44163</v>
+      </c>
+      <c r="C50">
+        <v>90</v>
+      </c>
+      <c r="D50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>193</v>
+      </c>
+      <c r="B51" s="3">
+        <v>44164</v>
+      </c>
+      <c r="C51">
+        <v>90</v>
+      </c>
+      <c r="D51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="3">
+        <v>44165</v>
+      </c>
+      <c r="C52">
+        <v>60</v>
+      </c>
+      <c r="D52" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="3">
+        <v>44165</v>
+      </c>
+      <c r="C53">
+        <v>40</v>
+      </c>
+      <c r="D53" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" s="3">
+        <v>44165</v>
+      </c>
+      <c r="C54">
+        <v>150</v>
+      </c>
+      <c r="D54" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3902,21 +4000,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:XFC68"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="16383" width="0" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="7.44140625" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="7.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -4749,6 +4847,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4974,26 +5091,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5011,30 +5135,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
demo 2 + logboek
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\NerdyGadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6001EDDF-D9E1-4AAD-86BB-AFDFF864A19F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0E8212-FA07-4677-BBB6-7EE798943B8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="205">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -780,8 +780,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D52" totalsRowShown="0">
-  <autoFilter ref="A9:D52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D54" totalsRowShown="0">
+  <autoFilter ref="A9:D54" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D45">
     <sortCondition ref="B9:B45"/>
   </sortState>
@@ -809,8 +809,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1572345" displayName="Table1572345" ref="A9:D72" totalsRowShown="0">
-  <autoFilter ref="A9:D72" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1572345" displayName="Table1572345" ref="A9:D74" totalsRowShown="0">
+  <autoFilter ref="A9:D74" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D67">
     <sortCondition ref="B9:B67"/>
   </sortState>
@@ -825,8 +825,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15723456" displayName="Table15723456" ref="A9:D54" totalsRowShown="0">
-  <autoFilter ref="A9:D54" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table15723456" displayName="Table15723456" ref="A9:D56" totalsRowShown="0">
+  <autoFilter ref="A9:D56" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Datum"/>
@@ -838,8 +838,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D68" totalsRowShown="0">
-  <autoFilter ref="A9:D68" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D70" totalsRowShown="0">
+  <autoFilter ref="A9:D70" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -1171,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -1230,7 +1230,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C153)/60</f>
-        <v>61.25</v>
+        <v>62.75</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C153)/60)</f>
-        <v>106.75</v>
+        <v>105.25</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1784,6 +1784,20 @@
       </c>
       <c r="D52" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" s="3">
+        <v>44166</v>
+      </c>
+      <c r="C53">
+        <v>90</v>
+      </c>
+      <c r="D53" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1806,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView view="pageLayout" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -2482,10 +2496,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:XFC72"/>
+  <dimension ref="A1:XFC74"/>
   <sheetViews>
     <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+      <selection activeCell="A73" sqref="A73:D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -2539,7 +2553,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C155)/60</f>
-        <v>88.083333333333329</v>
+        <v>90.083333333333329</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -2551,7 +2565,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C155)/60)</f>
-        <v>79.916666666666671</v>
+        <v>77.916666666666671</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -3377,6 +3391,34 @@
       </c>
       <c r="C72">
         <v>60</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="3">
+        <v>44166</v>
+      </c>
+      <c r="C73">
+        <v>60</v>
+      </c>
+      <c r="D73" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>203</v>
+      </c>
+      <c r="B74" s="3">
+        <v>44166</v>
+      </c>
+      <c r="C74">
+        <v>60</v>
+      </c>
+      <c r="D74" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3397,10 +3439,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -3453,7 +3495,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C154)/60</f>
-        <v>63.25</v>
+        <v>64.75</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -3465,7 +3507,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C154)/60)</f>
-        <v>104.75</v>
+        <v>103.25</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4037,6 +4079,20 @@
       </c>
       <c r="D54" t="s">
         <v>196</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>203</v>
+      </c>
+      <c r="B55" s="3">
+        <v>44166</v>
+      </c>
+      <c r="C55">
+        <v>90</v>
+      </c>
+      <c r="D55" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -4058,10 +4114,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:XFC68"/>
+  <dimension ref="A1:XFC70"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4123,7 +4179,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C153)/60)</f>
-        <v>86.833333333333329</v>
+        <v>84.333333333333329</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -4887,6 +4943,34 @@
       </c>
       <c r="D68" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>201</v>
+      </c>
+      <c r="B69" s="3">
+        <v>44166</v>
+      </c>
+      <c r="C69">
+        <v>60</v>
+      </c>
+      <c r="D69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>203</v>
+      </c>
+      <c r="B70" s="3">
+        <v>44166</v>
+      </c>
+      <c r="C70">
+        <v>90</v>
+      </c>
+      <c r="D70" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -4907,25 +4991,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5151,33 +5216,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5195,4 +5253,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
tijdschriftformulier & powerpoint demo
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projects\nerdygadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\NerdyGadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E28B178-7B9B-4313-A5F7-88AA618D947C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBE39B7-D81F-407F-8615-08339E12A4E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1680" windowWidth="25440" windowHeight="15540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="218">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -677,6 +677,24 @@
   </si>
   <si>
     <t>sendMail.php meermaals geïncluded. Meermaalse verwijderd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bezig met de code </t>
+  </si>
+  <si>
+    <t>Geprobeerd de customer service te maken, niet gelukt vraag morgen hulp van anderen</t>
+  </si>
+  <si>
+    <t>Start gemaakt met securityOpdracht.  Demo powerpoint gemaakt &amp; uitlogknop gemaakt</t>
+  </si>
+  <si>
+    <t>Start gemaakt met securityOpdracht. stijlen knoppen en versturen mail voor klantservice, powerpoint voor de demo gemaakt.</t>
+  </si>
+  <si>
+    <t>Securityverslag</t>
+  </si>
+  <si>
+    <t>KBS op locatie via teams</t>
   </si>
 </sst>
 </file>
@@ -817,8 +835,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15723" displayName="Table15723" ref="A9:D56" totalsRowShown="0">
-  <autoFilter ref="A9:D56" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15723" displayName="Table15723" ref="A9:D59" totalsRowShown="0">
+  <autoFilter ref="A9:D59" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Datum"/>
@@ -859,8 +877,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D70" totalsRowShown="0">
-  <autoFilter ref="A9:D70" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D71" totalsRowShown="0">
+  <autoFilter ref="A9:D71" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -1192,22 +1210,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A51" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView view="pageLayout" topLeftCell="A37" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1251,7 +1269,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C153)/60</f>
-        <v>62.75</v>
+        <v>64.25</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1263,7 +1281,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C153)/60)</f>
-        <v>105.25</v>
+        <v>103.75</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1819,6 +1837,20 @@
       </c>
       <c r="D53" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>217</v>
+      </c>
+      <c r="B54" s="3">
+        <v>44168</v>
+      </c>
+      <c r="C54">
+        <v>90</v>
+      </c>
+      <c r="D54" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1839,22 +1871,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView view="pageLayout" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="51.109375" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.140625" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1927,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C152)/60</f>
-        <v>71.666666666666671</v>
+        <v>76.916666666666671</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1907,7 +1939,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C152)/60)</f>
-        <v>96.333333333333329</v>
+        <v>91.083333333333329</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2497,6 +2529,48 @@
       </c>
       <c r="D56" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" s="3">
+        <v>44167</v>
+      </c>
+      <c r="C57">
+        <v>120</v>
+      </c>
+      <c r="D57" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="3">
+        <v>44168</v>
+      </c>
+      <c r="C58">
+        <v>180</v>
+      </c>
+      <c r="D58" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>210</v>
+      </c>
+      <c r="B59" s="3">
+        <v>44168</v>
+      </c>
+      <c r="C59">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -2519,21 +2593,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFC78"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
-    <col min="5" max="16383" width="9.109375" hidden="1"/>
-    <col min="16384" max="16384" width="0.109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" customWidth="1"/>
+    <col min="5" max="16383" width="9.140625" hidden="1"/>
+    <col min="16384" max="16384" width="0.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -2697,7 +2771,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2">
+    <row r="18" spans="1:4" ht="45">
       <c r="A18" s="7" t="s">
         <v>43</v>
       </c>
@@ -2711,7 +2785,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.8">
+    <row r="19" spans="1:4" ht="30">
       <c r="A19" s="7" t="s">
         <v>42</v>
       </c>
@@ -2894,7 +2968,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="28.8">
+    <row r="34" spans="1:4" ht="30">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -3518,20 +3592,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView view="pageLayout" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4191,23 +4265,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:XFC70"/>
+  <dimension ref="A1:XFC71"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.44140625" customWidth="1"/>
-    <col min="4" max="4" width="41.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
     <col min="5" max="16383" width="0" hidden="1" customWidth="1"/>
-    <col min="16384" max="16384" width="7.44140625" hidden="1" customWidth="1"/>
+    <col min="16384" max="16384" width="7.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.8">
+    <row r="1" spans="1:4" ht="26.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -4246,6 +4320,10 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B6">
+        <f>SUM(C10:C186)/60</f>
+        <v>86.666666666666671</v>
+      </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -4256,7 +4334,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C153)/60)</f>
-        <v>84.333333333333329</v>
+        <v>81.333333333333329</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -5048,6 +5126,20 @@
       </c>
       <c r="D70" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="3">
+        <v>44168</v>
+      </c>
+      <c r="C71">
+        <v>180</v>
+      </c>
+      <c r="D71" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -5068,25 +5160,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5312,33 +5385,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5356,4 +5422,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
logboek en footer (niet gelukt)
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FB3AFD-7D4A-4162-92FD-1B598D07DD0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463B993C-2BCD-49DB-AE76-837614B4B1A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="276">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -863,6 +863,12 @@
   </si>
   <si>
     <t>Alle data van een order wordt nu in de juiste tabellen in de database gezet, behalve discount.</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Geprobeerd de footer niet te laten plakken aan de onderkant. Heel wat manieren geprobeerd maar niet gelukt</t>
   </si>
 </sst>
 </file>
@@ -1085,8 +1091,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D91" totalsRowShown="0">
-  <autoFilter ref="A9:D91" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157" displayName="Table157" ref="A9:D92" totalsRowShown="0">
+  <autoFilter ref="A9:D92" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Activiteit"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Datum"/>
@@ -3170,7 +3176,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:XFC101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A79" workbookViewId="0">
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="D99" sqref="A99:D99"/>
     </sheetView>
   </sheetViews>
@@ -5367,10 +5373,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:XFC91"/>
+  <dimension ref="A1:XFC92"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5424,7 +5430,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C186)/60</f>
-        <v>126.91666666666667</v>
+        <v>128.16666666666666</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -5436,7 +5442,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C153)/60)</f>
-        <v>41.083333333333329</v>
+        <v>39.833333333333343</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -6513,6 +6519,20 @@
       </c>
       <c r="D91" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>274</v>
+      </c>
+      <c r="B92" s="3">
+        <v>44182</v>
+      </c>
+      <c r="C92">
+        <v>75</v>
+      </c>
+      <c r="D92" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -6533,25 +6553,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6777,33 +6778,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6821,4 +6815,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Password Policy en op signup.php variables Engels gemaakt
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets-master\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFC0701-1EE5-43EC-B627-DDB92DF01540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9824697-561A-41EB-9D5D-C7436529E429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="296">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -923,6 +923,12 @@
   </si>
   <si>
     <t>Nabespreken Demo + weekverslag</t>
+  </si>
+  <si>
+    <t>Password check afgemaakt, nu checkt deze doormiddel van een regex op; minimaal 1 uppercase, lowercase, number en of het wachtwoord minimaal 8 tekens bevat</t>
+  </si>
+  <si>
+    <t>Password Policy + variables Engels gemaakt</t>
   </si>
 </sst>
 </file>
@@ -1082,9 +1088,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1100,8 +1106,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D76" totalsRowShown="0">
-  <autoFilter ref="A9:D76" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D77" totalsRowShown="0">
+  <autoFilter ref="A9:D77" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D45">
     <sortCondition ref="B9:B45"/>
   </sortState>
@@ -1171,7 +1177,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1491,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -1550,7 +1556,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C161)/60</f>
-        <v>107.58333333333333</v>
+        <v>108.83333333333333</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1562,7 +1568,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C161)/60)</f>
-        <v>60.416666666666671</v>
+        <v>59.166666666666671</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2426,6 +2432,65 @@
       <c r="C76">
         <v>40</v>
       </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>295</v>
+      </c>
+      <c r="B77" s="3">
+        <v>44184</v>
+      </c>
+      <c r="C77">
+        <v>75</v>
+      </c>
+      <c r="D77" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7028,25 +7093,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7272,33 +7318,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7316,4 +7355,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
variables Engels gemaakt zie aantekeningen
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets-master\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9824697-561A-41EB-9D5D-C7436529E429}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024FBBD9-135D-46FB-B0E1-B90E4EA1CF3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="298">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -929,6 +929,12 @@
   </si>
   <si>
     <t>Password Policy + variables Engels gemaakt</t>
+  </si>
+  <si>
+    <t>Variables veranderen naar engels</t>
+  </si>
+  <si>
+    <t>variables veranderd in de volgende bestanden; cart.php, customerservice.php, export.php, index.php, login.php, order.php, pay.php, processingOrder.php, sendmail.php</t>
   </si>
 </sst>
 </file>
@@ -1106,8 +1112,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D77" totalsRowShown="0">
-  <autoFilter ref="A9:D77" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1572" displayName="Table1572" ref="A9:D78" totalsRowShown="0">
+  <autoFilter ref="A9:D78" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:D45">
     <sortCondition ref="B9:B45"/>
   </sortState>
@@ -1499,8 +1505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView view="pageLayout" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -1556,7 +1562,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C161)/60</f>
-        <v>108.83333333333333</v>
+        <v>107.58333333333333</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -1568,7 +1574,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C161)/60)</f>
-        <v>59.166666666666671</v>
+        <v>60.416666666666671</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -2432,23 +2438,6 @@
       <c r="C76">
         <v>40</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" t="s">
-        <v>295</v>
-      </c>
-      <c r="B77" s="3">
-        <v>44184</v>
-      </c>
-      <c r="C77">
-        <v>75</v>
-      </c>
-      <c r="D77" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="B78" s="3"/>
     </row>
     <row r="79" spans="1:4">
       <c r="B79" s="3"/>
@@ -2512,7 +2501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A58" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A80" sqref="A80:D80"/>
     </sheetView>
   </sheetViews>
@@ -4918,8 +4907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A49" zoomScale="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:D67"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -4972,7 +4961,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C177)/60</f>
-        <v>106.75</v>
+        <v>109.41666666666667</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -4984,7 +4973,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C177)/60)</f>
-        <v>61.25</v>
+        <v>58.583333333333329</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -5779,8 +5768,33 @@
         <v>40</v>
       </c>
     </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>295</v>
+      </c>
+      <c r="B68" s="3">
+        <v>44184</v>
+      </c>
+      <c r="C68">
+        <v>60</v>
+      </c>
+      <c r="D68" t="s">
+        <v>294</v>
+      </c>
+    </row>
     <row r="69" spans="1:4">
-      <c r="B69" s="3"/>
+      <c r="A69" t="s">
+        <v>296</v>
+      </c>
+      <c r="B69" s="3">
+        <v>44184</v>
+      </c>
+      <c r="C69">
+        <v>100</v>
+      </c>
+      <c r="D69" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="70" spans="1:4">
       <c r="B70" s="3"/>
@@ -7093,6 +7107,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010031DCE2413392E94399C66D8B3C6C85EE" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="e39e5be6c3b6c984bf8187e86b359ac0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xmlns:ns3="7178be8b-d0ef-4995-97d9-396f4bad9a56" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ced390a3fc2668719c5d57d8ce08db4" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7318,26 +7351,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
+    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="e7647ff1-e2f7-42a1-a68c-3c96587cf758" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FAC8759-EB35-489F-BF7F-6A43D48E2DBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7355,30 +7395,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC37EE7-F303-4AA4-9912-15E2B786CD45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{241D7108-AF27-4EE7-8B56-8DE5736E6E29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e7647ff1-e2f7-42a1-a68c-3c96587cf758"/>
-    <ds:schemaRef ds:uri="7178be8b-d0ef-4995-97d9-396f4bad9a56"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
functioneel ontwerp aangevuld en opgemaakt
</commit_message>
<xml_diff>
--- a/Documenten/Tijdschriftformulier.xlsx
+++ b/Documenten/Tijdschriftformulier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\nerdygadgets\Documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\NerdyGadgets\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37706B0E-AB18-40F8-8DB9-53AD97929D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F5D29A-D951-44E3-A0B4-05B4AA7EE04C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P1 - Anastasia" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="304">
   <si>
     <t>Tijdschrijfformulier</t>
   </si>
@@ -950,6 +950,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zelfevaluatie </t>
+  </si>
+  <si>
+    <t>Functioneel ontwerp aangevuld</t>
   </si>
 </sst>
 </file>
@@ -1109,9 +1112,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1198,7 +1201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4966,8 +4969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:D70"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
@@ -5020,7 +5023,7 @@
       </c>
       <c r="B6">
         <f>SUM(C10:C177)/60</f>
-        <v>110.91666666666667</v>
+        <v>111.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -5032,7 +5035,7 @@
       </c>
       <c r="B7">
         <f>(2*3*28)-(SUM(C10:C177)/60)</f>
-        <v>57.083333333333329</v>
+        <v>56.5</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -5867,7 +5870,15 @@
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="B71" s="3"/>
+      <c r="A71" t="s">
+        <v>303</v>
+      </c>
+      <c r="B71" s="3">
+        <v>44187</v>
+      </c>
+      <c r="C71">
+        <v>35</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
       <c r="B72" s="3"/>
@@ -5943,7 +5954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:XFC99"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A82" workbookViewId="0">
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A82" workbookViewId="0">
       <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>

</xml_diff>